<commit_message>
Added annif eval dataset ggc3
ggc3 dataset is much smaller, because of form keywords (vormtrefworden) being removed.
</commit_message>
<xml_diff>
--- a/annif_uitkomsten.xlsx
+++ b/annif_uitkomsten.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haighton_macbook/Desktop/Annif/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haighton_macbook/Desktop/Projects/KB/automatisch_onderwerp_ontsluiting/documenten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B274A5-9DFB-E641-816D-16F6476E4AC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF2F496-A7B1-C747-9ED7-37D650588BBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="24820" windowHeight="15000" xr2:uid="{48357401-DF52-0D42-B867-2D5831CDBB9F}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="25600" windowHeight="16000" xr2:uid="{48357401-DF52-0D42-B867-2D5831CDBB9F}"/>
   </bookViews>
   <sheets>
     <sheet name="Evaluatie_modellen" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="252">
   <si>
     <t>Precision (doc avg):</t>
   </si>
@@ -482,6 +482,306 @@
   </si>
   <si>
     <t>fasttext-brinkman (lim20_ep200)</t>
+  </si>
+  <si>
+    <t>0.07569331158238173</t>
+  </si>
+  <si>
+    <t>0.6567427949972812</t>
+  </si>
+  <si>
+    <t>0.13428279170530394</t>
+  </si>
+  <si>
+    <t>0.004047189024944168</t>
+  </si>
+  <si>
+    <t>0.006990727429274436</t>
+  </si>
+  <si>
+    <t>0.004240094397716624</t>
+  </si>
+  <si>
+    <t>0.5792759051186017</t>
+  </si>
+  <si>
+    <t>0.13389121338912133</t>
+  </si>
+  <si>
+    <t>0.49880563066253164</t>
+  </si>
+  <si>
+    <t>0.48103970935988066</t>
+  </si>
+  <si>
+    <t>0.3295269168026101</t>
+  </si>
+  <si>
+    <t>0.20228384991843393</t>
+  </si>
+  <si>
+    <t>0.13833605220228387</t>
+  </si>
+  <si>
+    <t>0.4318038355791462</t>
+  </si>
+  <si>
+    <t>dataset</t>
+  </si>
+  <si>
+    <t>summaries (ggc1)</t>
+  </si>
+  <si>
+    <t>summaries and titles (ggc2)</t>
+  </si>
+  <si>
+    <t>0.10121248608198037</t>
+  </si>
+  <si>
+    <t>0.5028548123980424</t>
+  </si>
+  <si>
+    <t>0.15782981745461355</t>
+  </si>
+  <si>
+    <t>0.0008344820729150113</t>
+  </si>
+  <si>
+    <t>0.002701965099620114</t>
+  </si>
+  <si>
+    <t>0.0011161286908728746</t>
+  </si>
+  <si>
+    <t>0.06359149582384206</t>
+  </si>
+  <si>
+    <t>0.418227215980025</t>
+  </si>
+  <si>
+    <t>0.11039710001647718</t>
+  </si>
+  <si>
+    <t>0.42305549367628054</t>
+  </si>
+  <si>
+    <t>0.4081982956186036</t>
+  </si>
+  <si>
+    <t>0.33442088091353994</t>
+  </si>
+  <si>
+    <t>0.16421968461120173</t>
+  </si>
+  <si>
+    <t>0.12444263186514411</t>
+  </si>
+  <si>
+    <t>0.39142856181298796</t>
+  </si>
+  <si>
+    <t>0.07732463295269167</t>
+  </si>
+  <si>
+    <t>0.6706090266449157</t>
+  </si>
+  <si>
+    <t>0.13717467958903523</t>
+  </si>
+  <si>
+    <t>0.004004294236221686</t>
+  </si>
+  <si>
+    <t>0.007079590558776096</t>
+  </si>
+  <si>
+    <t>0.00427077613027303</t>
+  </si>
+  <si>
+    <t>0.07732463295269168</t>
+  </si>
+  <si>
+    <t>0.5917602996254682</t>
+  </si>
+  <si>
+    <t>0.13677679988457653</t>
+  </si>
+  <si>
+    <t>0.5400695953137147</t>
+  </si>
+  <si>
+    <t>0.5245916706780286</t>
+  </si>
+  <si>
+    <t>0.39804241435562804</t>
+  </si>
+  <si>
+    <t>0.20717781402936378</t>
+  </si>
+  <si>
+    <t>0.14192495921696574</t>
+  </si>
+  <si>
+    <t>0.48363915197240664</t>
+  </si>
+  <si>
+    <t>0.05734265734265734</t>
+  </si>
+  <si>
+    <t>0.43589743589743585</t>
+  </si>
+  <si>
+    <t>0.09962997375584788</t>
+  </si>
+  <si>
+    <t>0.004223129254272983</t>
+  </si>
+  <si>
+    <t>0.0068591526995544095</t>
+  </si>
+  <si>
+    <t>0.004436873521374578</t>
+  </si>
+  <si>
+    <t>0.057342657342657345</t>
+  </si>
+  <si>
+    <t>0.3877068557919622</t>
+  </si>
+  <si>
+    <t>0.0999086201644837</t>
+  </si>
+  <si>
+    <t>0.1576756576756577</t>
+  </si>
+  <si>
+    <t>0.35215596865133314</t>
+  </si>
+  <si>
+    <t>0.3365088031123186</t>
+  </si>
+  <si>
+    <t>0.2867132867132867</t>
+  </si>
+  <si>
+    <t>0.14219114219114218</t>
+  </si>
+  <si>
+    <t>0.10209790209790211</t>
+  </si>
+  <si>
+    <t>0.30310701593612005</t>
+  </si>
+  <si>
+    <t>F1@5:</t>
+  </si>
+  <si>
+    <t>summaries and titles no form (ggc3)</t>
+  </si>
+  <si>
+    <t>summaries and titles no form (geen vormtrefwoorden i.e. kleine set) (ggc3)</t>
+  </si>
+  <si>
+    <t>NOTITES</t>
+  </si>
+  <si>
+    <t>Lagere recall, komt dit door gebruik kleinere dataset (5710 in ggc3 v 12243 in ggc1 en ggc2)</t>
+  </si>
+  <si>
+    <t>0.025524475524475527</t>
+  </si>
+  <si>
+    <t>0.19143356643356643</t>
+  </si>
+  <si>
+    <t>0.044254696352598454</t>
+  </si>
+  <si>
+    <t>0.001022761882033663</t>
+  </si>
+  <si>
+    <t>0.0028640254364621603</t>
+  </si>
+  <si>
+    <t>0.0013811605599035573</t>
+  </si>
+  <si>
+    <t>0.025569176882661998</t>
+  </si>
+  <si>
+    <t>0.17257683215130024</t>
+  </si>
+  <si>
+    <t>0.04453935326418548</t>
+  </si>
+  <si>
+    <t>0.0662948162948163</t>
+  </si>
+  <si>
+    <t>0.14018330333980838</t>
+  </si>
+  <si>
+    <t>0.13100342441816795</t>
+  </si>
+  <si>
+    <t>0.0944055944055944</t>
+  </si>
+  <si>
+    <t>0.05011655011655011</t>
+  </si>
+  <si>
+    <t>0.04265734265734266</t>
+  </si>
+  <si>
+    <t>0.11795614019141583</t>
+  </si>
+  <si>
+    <t>0.0562937062937063</t>
+  </si>
+  <si>
+    <t>0.42657342657342656</t>
+  </si>
+  <si>
+    <t>0.09773094038828306</t>
+  </si>
+  <si>
+    <t>0.003988741187078641</t>
+  </si>
+  <si>
+    <t>0.0067121304652688245</t>
+  </si>
+  <si>
+    <t>0.004291582197421854</t>
+  </si>
+  <si>
+    <t>0.056293706293706294</t>
+  </si>
+  <si>
+    <t>0.3806146572104019</t>
+  </si>
+  <si>
+    <t>0.09808102345415778</t>
+  </si>
+  <si>
+    <t>0.1531801531801532</t>
+  </si>
+  <si>
+    <t>0.3192570143916398</t>
+  </si>
+  <si>
+    <t>0.30201441416115327</t>
+  </si>
+  <si>
+    <t>0.2097902097902098</t>
+  </si>
+  <si>
+    <t>0.13752913752913754</t>
+  </si>
+  <si>
+    <t>0.0993006993006993</t>
+  </si>
+  <si>
+    <t>0.2668372851962632</t>
   </si>
 </sst>
 </file>
@@ -492,7 +792,7 @@
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
     <numFmt numFmtId="165" formatCode="0.00000000000000000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -514,6 +814,14 @@
       <name val="Menlo"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -523,7 +831,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -540,11 +848,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -575,8 +893,31 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -843,376 +1184,566 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00829E8A-756A-304D-A992-45393C8D1720}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="J2" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="J3" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="J4" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>200</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E5" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+      <c r="J5" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="M5" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C6" s="6">
         <v>5.775638327E-5</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E6" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="J6" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="M6" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="J7" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C8" s="6">
         <v>9.8788284670000006E-5</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E8" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="J8" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E9" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="J9" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="M9" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E10" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="J10" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="M10" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E11" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="J11" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="J12" s="16"/>
+      <c r="M12" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>19</v>
@@ -1238,240 +1769,507 @@
       <c r="I13" s="6" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H16" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I16" s="6" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="J16" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I17" s="6" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="J17" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C18" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="J18" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="M18" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B19" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G19" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I19" s="6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="J19" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B20" s="5">
         <v>439</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C20" s="5">
         <v>349</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D20" s="5">
         <v>448</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E20" s="12">
         <v>427</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F20" s="5">
         <v>439</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G20" s="5">
         <v>328</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H20" s="5">
         <v>331</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I20" s="5">
         <v>318</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="J20" s="17">
+        <v>464</v>
+      </c>
+      <c r="K20" s="5">
+        <v>335</v>
+      </c>
+      <c r="L20" s="5">
+        <v>474</v>
+      </c>
+      <c r="M20" s="17">
+        <v>164</v>
+      </c>
+      <c r="N20" s="5">
+        <v>73</v>
+      </c>
+      <c r="O20" s="5">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B21" s="5">
         <v>5691</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C21" s="5">
         <v>5774</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D21" s="5">
         <v>5682</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E21" s="12">
         <v>5703</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F21" s="5">
         <v>5691</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G21" s="5">
         <v>5337</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H21" s="5">
         <v>5147</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I21" s="5">
         <v>5036</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="J21" s="17">
+        <v>5666</v>
+      </c>
+      <c r="K21" s="5">
+        <v>4933</v>
+      </c>
+      <c r="L21" s="5">
+        <v>5656</v>
+      </c>
+      <c r="M21" s="17">
+        <v>2696</v>
+      </c>
+      <c r="N21" s="5">
+        <v>2782</v>
+      </c>
+      <c r="O21" s="5">
+        <v>2699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B22" s="5">
         <v>362</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C22" s="5">
         <v>452</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D22" s="5">
         <v>353</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E22" s="12">
         <v>374</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F22" s="5">
         <v>362</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G22" s="5">
         <v>473</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H22" s="5">
         <v>470</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I22" s="5">
         <v>483</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="J22" s="17">
+        <v>337</v>
+      </c>
+      <c r="K22" s="5">
+        <v>466</v>
+      </c>
+      <c r="L22" s="5">
+        <v>327</v>
+      </c>
+      <c r="M22" s="17">
+        <v>259</v>
+      </c>
+      <c r="N22" s="5">
+        <v>350</v>
+      </c>
+      <c r="O22" s="5">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B23" s="5">
         <v>613</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C23" s="5">
         <v>613</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D23" s="5">
         <v>613</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E23" s="12">
         <v>613</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F23" s="5">
         <v>613</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G23" s="5">
         <v>613</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H23" s="5">
         <v>613</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I23" s="5">
         <v>613</v>
       </c>
+      <c r="J23" s="17">
+        <v>613</v>
+      </c>
+      <c r="K23" s="5">
+        <v>613</v>
+      </c>
+      <c r="L23" s="5">
+        <v>613</v>
+      </c>
+      <c r="M23" s="18">
+        <v>286</v>
+      </c>
+      <c r="N23" s="5">
+        <v>286</v>
+      </c>
+      <c r="O23" s="5">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="M25" s="21" t="s">
+        <v>219</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" xr:uid="{B5CE542B-4A88-B249-81D8-C6F32D47B645}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -1482,7 +2280,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>